<commit_message>
add validation for document
</commit_message>
<xml_diff>
--- a/downloads/timesheet_787169317.xlsx
+++ b/downloads/timesheet_787169317.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS TUF\Desktop\SeleniumProject\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB11408A-79D2-4572-8FB8-32DADF16C4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DE0A39-303F-4DAF-9A56-EA26D11AE789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7618A666-F6FF-4AC6-8889-F663CE4131DC}"/>
   </bookViews>
@@ -516,14 +516,14 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.21875" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="3" max="3" width="29.77734375" customWidth="1"/>
     <col min="4" max="4" width="16.44140625" customWidth="1"/>
     <col min="5" max="5" width="32.109375" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" customWidth="1"/>

</xml_diff>